<commit_message>
added more description to Twinkle.ipynb
</commit_message>
<xml_diff>
--- a/sedDatFileDescription.xlsx
+++ b/sedDatFileDescription.xlsx
@@ -416,18 +416,6 @@
     <t>mag</t>
   </si>
   <si>
-    <t>HIP26062</t>
-  </si>
-  <si>
-    <t>HD_36546</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>NextGen</t>
   </si>
   <si>
@@ -476,10 +464,22 @@
     <t>Applicable with plot_sed.py</t>
   </si>
   <si>
-    <t>HPACS160, HPACS100, Akari90</t>
-  </si>
-  <si>
     <t>Add only when necessary</t>
+  </si>
+  <si>
+    <t>Star_ID1</t>
+  </si>
+  <si>
+    <t>Star_ID2</t>
+  </si>
+  <si>
+    <t>A2V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>HPACS160,HPACS100,Akari90</t>
   </si>
 </sst>
 </file>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -634,6 +634,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -919,10 +920,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:BG58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="132" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,11 +937,12 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -957,13 +962,13 @@
         <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -977,10 +982,10 @@
         <v>125</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>60</v>
@@ -988,8 +993,9 @@
       <c r="H2" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1003,10 +1009,10 @@
         <v>125</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>61</v>
@@ -1014,8 +1020,10 @@
       <c r="H3" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L3" s="10"/>
+      <c r="BG3" s="12"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1029,10 +1037,10 @@
         <v>125</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>60</v>
@@ -1041,7 +1049,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1055,10 +1063,10 @@
         <v>125</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>61</v>
@@ -1067,7 +1075,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1081,10 +1089,10 @@
         <v>125</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>60</v>
@@ -1093,7 +1101,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1107,7 +1115,7 @@
         <v>125</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F7" s="10" t="b">
         <v>0</v>
@@ -1119,7 +1127,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1133,10 +1141,10 @@
         <v>125</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>60</v>
@@ -1145,7 +1153,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1159,7 +1167,7 @@
         <v>126</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F9" s="10">
         <v>5000</v>
@@ -1171,7 +1179,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1185,7 +1193,7 @@
         <v>127</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="10">
         <v>40</v>
@@ -1197,7 +1205,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1231,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1240,7 +1248,7 @@
         <v>125</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>61</v>
@@ -1249,7 +1257,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1260,13 +1268,13 @@
         <v>122</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F13" s="10">
-        <v>8.7799999999999994</v>
+        <v>15.6</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>60</v>
@@ -1275,7 +1283,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1286,13 +1294,13 @@
         <v>122</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F14" s="10">
-        <v>0.61</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>60</v>
@@ -1301,7 +1309,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>125</v>
       </c>
       <c r="F15" s="10">
-        <v>5.5E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>60</v>
@@ -1327,7 +1335,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1352,7 @@
         <v>125</v>
       </c>
       <c r="F16" s="10">
-        <v>8.9999999999999993E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>60</v>
@@ -1370,7 +1378,7 @@
         <v>125</v>
       </c>
       <c r="F17" s="10">
-        <v>8.2000000000000003E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>61</v>
@@ -1396,7 +1404,7 @@
         <v>125</v>
       </c>
       <c r="F18" s="10">
-        <v>1.8601075000000002E-2</v>
+        <v>1.6643317000000001E-2</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>61</v>
@@ -1422,7 +1430,7 @@
         <v>125</v>
       </c>
       <c r="F19" s="10">
-        <v>8.2000000000000003E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>61</v>
@@ -1448,7 +1456,7 @@
         <v>125</v>
       </c>
       <c r="F20" s="10">
-        <v>7.02</v>
+        <v>5.242</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>60</v>
@@ -1474,7 +1482,7 @@
         <v>125</v>
       </c>
       <c r="F21" s="10">
-        <v>0.01</v>
+        <v>9.9739560000000008E-3</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>60</v>
@@ -1500,7 +1508,7 @@
         <v>125</v>
       </c>
       <c r="F22" s="10">
-        <v>6.95</v>
+        <v>5.17</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>60</v>
@@ -1526,7 +1534,7 @@
         <v>125</v>
       </c>
       <c r="F23" s="10">
-        <v>0.01</v>
+        <v>9.9236989999999994E-3</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>60</v>
@@ -1552,7 +1560,7 @@
         <v>125</v>
       </c>
       <c r="F24" s="10">
-        <v>6.9619999999999997</v>
+        <v>5.1749999999999998</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>61</v>
@@ -1578,7 +1586,7 @@
         <v>125</v>
       </c>
       <c r="F25" s="10">
-        <v>1.0999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>61</v>
@@ -1604,7 +1612,7 @@
         <v>125</v>
       </c>
       <c r="F26" s="10">
-        <v>7.0439999999999996</v>
+        <v>5.2610000000000001</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>61</v>
@@ -1630,7 +1638,7 @@
         <v>125</v>
       </c>
       <c r="F27" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>61</v>
@@ -1656,7 +1664,7 @@
         <v>125</v>
       </c>
       <c r="F28" s="10">
-        <v>6.8449999999999998</v>
+        <v>5.085</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>60</v>
@@ -1682,7 +1690,7 @@
         <v>125</v>
       </c>
       <c r="F29" s="10">
-        <v>2.4E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>60</v>
@@ -1708,7 +1716,7 @@
         <v>125</v>
       </c>
       <c r="F30" s="10">
-        <v>6.9219999999999997</v>
+        <v>5.0570000000000004</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>60</v>
@@ -1734,7 +1742,7 @@
         <v>125</v>
       </c>
       <c r="F31" s="10">
-        <v>4.2000000000000003E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>60</v>
@@ -1760,7 +1768,7 @@
         <v>125</v>
       </c>
       <c r="F32" s="10">
-        <v>6.8150000000000004</v>
+        <v>4.9260000000000002</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>60</v>
@@ -1786,7 +1794,7 @@
         <v>125</v>
       </c>
       <c r="F33" s="10">
-        <v>2.3E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>60</v>
@@ -1812,7 +1820,7 @@
         <v>125</v>
       </c>
       <c r="F34" s="10">
-        <v>6.7910000000000004</v>
+        <v>4.9569999999999999</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>60</v>
@@ -1838,7 +1846,7 @@
         <v>125</v>
       </c>
       <c r="F35" s="10">
-        <v>3.5999999999999997E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>60</v>
@@ -1864,7 +1872,7 @@
         <v>125</v>
       </c>
       <c r="F36" s="10">
-        <v>6.7866736950000002</v>
+        <v>4.9297599410000004</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>60</v>
@@ -1890,7 +1898,7 @@
         <v>125</v>
       </c>
       <c r="F37" s="10">
-        <v>3.7999999999999999E-2</v>
+        <v>7.7210686000000001E-2</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>60</v>
@@ -1916,7 +1924,7 @@
         <v>125</v>
       </c>
       <c r="F38" s="10">
-        <v>6.7610000000000001</v>
+        <v>4.6340000000000003</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>60</v>
@@ -1942,7 +1950,7 @@
         <v>125</v>
       </c>
       <c r="F39" s="10">
-        <v>2.1000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>60</v>
@@ -1968,7 +1976,7 @@
         <v>125</v>
       </c>
       <c r="F40" s="10">
-        <v>6.7610000000000001</v>
+        <v>4.9389477810000004</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>60</v>
@@ -1994,7 +2002,7 @@
         <v>125</v>
       </c>
       <c r="F41" s="10">
-        <v>2.1000000000000001E-2</v>
+        <v>4.0660669000000003E-2</v>
       </c>
       <c r="G41" s="11" t="s">
         <v>60</v>
@@ -2020,7 +2028,7 @@
         <v>125</v>
       </c>
       <c r="F42" s="10">
-        <v>5.1260000000000003</v>
+        <v>4.9530000000000003</v>
       </c>
       <c r="G42" s="11" t="s">
         <v>60</v>
@@ -2046,7 +2054,7 @@
         <v>125</v>
       </c>
       <c r="F43" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>60</v>
@@ -2072,7 +2080,7 @@
         <v>125</v>
       </c>
       <c r="F44" s="10">
-        <v>5.1260000000000003</v>
+        <v>4.9530000000000003</v>
       </c>
       <c r="G44" s="11" t="s">
         <v>61</v>
@@ -2098,7 +2106,7 @@
         <v>125</v>
       </c>
       <c r="F45" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>61</v>
@@ -2124,7 +2132,7 @@
         <v>125</v>
       </c>
       <c r="F46" s="10">
-        <v>2.2829999999999999</v>
+        <v>4.8220000000000001</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>60</v>
@@ -2150,7 +2158,7 @@
         <v>125</v>
       </c>
       <c r="F47" s="10">
-        <v>1.7000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>60</v>
@@ -2176,7 +2184,7 @@
         <v>125</v>
       </c>
       <c r="F48" s="10">
-        <v>118.9844038</v>
+        <v>5</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>61</v>
@@ -2190,7 +2198,7 @@
         <v>45</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>120</v>
@@ -2202,13 +2210,13 @@
         <v>125</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>60</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2222,19 +2230,19 @@
         <v>122</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>125</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G50" s="11" t="s">
         <v>61</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2248,19 +2256,19 @@
         <v>122</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>125</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>61</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2274,19 +2282,19 @@
         <v>122</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>125</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>61</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2300,7 +2308,7 @@
         <v>122</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>125</v>
@@ -2312,7 +2320,7 @@
         <v>61</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2326,7 +2334,7 @@
         <v>122</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>125</v>
@@ -2338,7 +2346,7 @@
         <v>61</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2352,7 +2360,7 @@
         <v>122</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>125</v>
@@ -2364,7 +2372,7 @@
         <v>61</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2378,7 +2386,7 @@
         <v>122</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>125</v>
@@ -2390,7 +2398,7 @@
         <v>61</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2404,7 +2412,7 @@
         <v>122</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>125</v>
@@ -2416,7 +2424,7 @@
         <v>61</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2430,7 +2438,7 @@
         <v>122</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>125</v>
@@ -2442,10 +2450,11 @@
         <v>61</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>